<commit_message>
Results added and script testing
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sanchit\workspace\Bellman-Ford\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25516"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -51,10 +49,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -77,8 +91,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -86,7 +116,23 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="17">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -100,6 +146,827 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800"/>
+              <a:t>Uber Dataset 350 Nodes</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Online/Offline</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0547953345719426"/>
+                  <c:y val="0.0425269645608629"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:numFmt formatCode="#,##0.00000" sourceLinked="0"/>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$K$3:$T$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$4:$T$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.34370480721398</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.26327805810038</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.30486805719736</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.29710107749564</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.25498146200484</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.24970077963656</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.24621578355748</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.24239764811306</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.24880946355503</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.25025681183587</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Greedy/Offline</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$K$3:$T$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$5:$T$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.29282889768566</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.29282889768566</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.29282889768566</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.29282889768566</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.29282889768566</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.29282889768566</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.29282889768566</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.29282889768566</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.29282889768566</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.29282889768566</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2063765864"/>
+        <c:axId val="2072374744"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2063765864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Coefficient</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2072374744"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2072374744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Competetive Ratio</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2063765864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1200"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800"/>
+              <a:t>Synthetic Dataset 350 Nodes</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Online/Offline</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0547953345719426"/>
+                  <c:y val="0.0425269645608629"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:numFmt formatCode="#,##0.00000" sourceLinked="0"/>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$K$3:$T$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$7:$T$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.44221246006114</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.39431699855319</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.33599696674708</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.30752097755763</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.45483309096827</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.39195477506776</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.36457429789238</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.25749777322223</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.42843014032757</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.37163588865373</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Greedy/Offline</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$K$3:$T$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$8:$T$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.33682740305212</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.31430287514406</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.29165859867737</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.19712945639231</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.25842312748113</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.32610409708574</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.27124003804951</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.34078148458782</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.32059336365173</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.29930606218373</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2079802696"/>
+        <c:axId val="2079808104"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2079802696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Coefficient</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2079808104"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2079808104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Competetive Ratio</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2079802696"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1200"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -145,7 +1012,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -180,7 +1047,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -357,7 +1224,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -365,18 +1232,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Q33" sqref="Q33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -390,7 +1257,7 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -403,8 +1270,11 @@
       <c r="H2">
         <v>350</v>
       </c>
+      <c r="K2">
+        <v>350</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20">
       <c r="E3">
         <v>1</v>
       </c>
@@ -417,8 +1287,38 @@
       <c r="I3">
         <v>3</v>
       </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1.5</v>
+      </c>
+      <c r="M3">
+        <v>2</v>
+      </c>
+      <c r="N3">
+        <v>2.5</v>
+      </c>
+      <c r="O3">
+        <v>3</v>
+      </c>
+      <c r="P3">
+        <v>3.5</v>
+      </c>
+      <c r="Q3">
+        <v>4</v>
+      </c>
+      <c r="R3">
+        <v>5</v>
+      </c>
+      <c r="S3">
+        <v>10</v>
+      </c>
+      <c r="T3">
+        <v>25</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -428,6 +1328,9 @@
       <c r="C4">
         <v>1.2428908532482901</v>
       </c>
+      <c r="D4">
+        <v>1.0873758416972701</v>
+      </c>
       <c r="E4">
         <v>1.28817622422902</v>
       </c>
@@ -440,8 +1343,38 @@
       <c r="I4">
         <v>1.26739976341898</v>
       </c>
+      <c r="K4">
+        <v>1.3437048072139799</v>
+      </c>
+      <c r="L4">
+        <v>1.26327805810038</v>
+      </c>
+      <c r="M4">
+        <v>1.3048680571973601</v>
+      </c>
+      <c r="N4">
+        <v>1.29710107749564</v>
+      </c>
+      <c r="O4">
+        <v>1.2549814620048401</v>
+      </c>
+      <c r="P4">
+        <v>1.24970077963656</v>
+      </c>
+      <c r="Q4">
+        <v>1.2462157835574801</v>
+      </c>
+      <c r="R4">
+        <v>1.2423976481130601</v>
+      </c>
+      <c r="S4">
+        <v>1.24880946355503</v>
+      </c>
+      <c r="T4">
+        <v>1.2502568118358699</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -451,6 +1384,9 @@
       <c r="C5">
         <v>1.1289783577941599</v>
       </c>
+      <c r="D5">
+        <v>1.0873758416972701</v>
+      </c>
       <c r="E5">
         <v>1.31596413308198</v>
       </c>
@@ -463,8 +1399,38 @@
       <c r="I5">
         <v>1.2665229999671801</v>
       </c>
+      <c r="K5">
+        <v>1.2928288976856599</v>
+      </c>
+      <c r="L5">
+        <v>1.2928288976856599</v>
+      </c>
+      <c r="M5">
+        <v>1.2928288976856599</v>
+      </c>
+      <c r="N5">
+        <v>1.2928288976856599</v>
+      </c>
+      <c r="O5">
+        <v>1.2928288976856599</v>
+      </c>
+      <c r="P5">
+        <v>1.2928288976856599</v>
+      </c>
+      <c r="Q5">
+        <v>1.2928288976856599</v>
+      </c>
+      <c r="R5">
+        <v>1.2928288976856599</v>
+      </c>
+      <c r="S5">
+        <v>1.2928288976856599</v>
+      </c>
+      <c r="T5">
+        <v>1.2928288976856599</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -480,8 +1446,38 @@
       <c r="F7">
         <v>1.18535900554505</v>
       </c>
+      <c r="K7">
+        <v>1.4422124600611399</v>
+      </c>
+      <c r="L7">
+        <v>1.39431699855319</v>
+      </c>
+      <c r="M7">
+        <v>1.3359969667470799</v>
+      </c>
+      <c r="N7">
+        <v>1.30752097755763</v>
+      </c>
+      <c r="O7">
+        <v>1.4548330909682701</v>
+      </c>
+      <c r="P7">
+        <v>1.3919547750677601</v>
+      </c>
+      <c r="Q7">
+        <v>1.3645742978923801</v>
+      </c>
+      <c r="R7">
+        <v>1.2574977732222301</v>
+      </c>
+      <c r="S7">
+        <v>1.4284301403275701</v>
+      </c>
+      <c r="T7">
+        <v>1.3716358886537301</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -497,8 +1493,38 @@
       <c r="F8">
         <v>1.1862333464305901</v>
       </c>
+      <c r="K8">
+        <v>1.3368274030521199</v>
+      </c>
+      <c r="L8">
+        <v>1.31430287514406</v>
+      </c>
+      <c r="M8">
+        <v>1.2916585986773701</v>
+      </c>
+      <c r="N8">
+        <v>1.1971294563923101</v>
+      </c>
+      <c r="O8">
+        <v>1.2584231274811299</v>
+      </c>
+      <c r="P8">
+        <v>1.3261040970857401</v>
+      </c>
+      <c r="Q8">
+        <v>1.2712400380495099</v>
+      </c>
+      <c r="R8">
+        <v>1.3407814845878201</v>
+      </c>
+      <c r="S8">
+        <v>1.32059336365173</v>
+      </c>
+      <c r="T8">
+        <v>1.29930606218373</v>
+      </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -515,7 +1541,7 @@
         <v>1.0552545729212801</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -529,7 +1555,7 @@
         <v>1.1064544729224499</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -540,7 +1566,7 @@
         <v>1.10113980595296</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -551,7 +1577,7 @@
         <v>1.1002654650674299</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -562,7 +1588,7 @@
         <v>1.1779659898652199</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -579,5 +1605,12 @@
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added edge costs and numEdges
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25516"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sanchit\workspace\Bellman-Ford\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -227,8 +222,8 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-5.4795334571942599E-2"/>
-                  <c:y val="4.2526964560862898E-2"/>
+                  <c:x val="-0.0547953345719426"/>
+                  <c:y val="0.0425269645608629"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -274,34 +269,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -313,34 +308,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.3437048072139799</c:v>
+                  <c:v>1.34370480721398</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.26327805810038</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.3048680571973601</c:v>
+                  <c:v>1.30486805719736</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.29710107749564</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.2549814620048401</c:v>
+                  <c:v>1.25498146200484</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1.24970077963656</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.2462157835574801</c:v>
+                  <c:v>1.24621578355748</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.2423976481130601</c:v>
+                  <c:v>1.24239764811306</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1.24880946355503</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.2502568118358699</c:v>
+                  <c:v>1.25025681183587</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -374,34 +369,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -413,34 +408,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.2928288976856599</c:v>
+                  <c:v>1.29282889768566</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2928288976856599</c:v>
+                  <c:v>1.29282889768566</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.2928288976856599</c:v>
+                  <c:v>1.29282889768566</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2928288976856599</c:v>
+                  <c:v>1.29282889768566</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.2928288976856599</c:v>
+                  <c:v>1.29282889768566</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.2928288976856599</c:v>
+                  <c:v>1.29282889768566</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.2928288976856599</c:v>
+                  <c:v>1.29282889768566</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.2928288976856599</c:v>
+                  <c:v>1.29282889768566</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.2928288976856599</c:v>
+                  <c:v>1.29282889768566</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.2928288976856599</c:v>
+                  <c:v>1.29282889768566</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -457,11 +452,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="206626704"/>
-        <c:axId val="206621808"/>
+        <c:axId val="2074780904"/>
+        <c:axId val="2074786424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="206626704"/>
+        <c:axId val="2074780904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -490,7 +485,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="206621808"/>
+        <c:crossAx val="2074786424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -498,7 +493,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="206621808"/>
+        <c:axId val="2074786424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -528,7 +523,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="206626704"/>
+        <c:crossAx val="2074780904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -554,7 +549,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -622,8 +617,8 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-5.4795334571942599E-2"/>
-                  <c:y val="4.2526964560862898E-2"/>
+                  <c:x val="-0.0547953345719426"/>
+                  <c:y val="0.0425269645608629"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -669,34 +664,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -708,34 +703,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.4422124600611399</c:v>
+                  <c:v>1.44221246006114</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.39431699855319</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.3359969667470799</c:v>
+                  <c:v>1.33599696674708</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.30752097755763</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.4548330909682701</c:v>
+                  <c:v>1.45483309096827</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.3919547750677601</c:v>
+                  <c:v>1.39195477506776</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3645742978923801</c:v>
+                  <c:v>1.36457429789238</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.2574977732222301</c:v>
+                  <c:v>1.25749777322223</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.4284301403275701</c:v>
+                  <c:v>1.42843014032757</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.3716358886537301</c:v>
+                  <c:v>1.37163588865373</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -769,34 +764,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -808,28 +803,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.3368274030521199</c:v>
+                  <c:v>1.33682740305212</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.31430287514406</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.2916585986773701</c:v>
+                  <c:v>1.29165859867737</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1971294563923101</c:v>
+                  <c:v>1.19712945639231</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.2584231274811299</c:v>
+                  <c:v>1.25842312748113</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.3261040970857401</c:v>
+                  <c:v>1.32610409708574</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.2712400380495099</c:v>
+                  <c:v>1.27124003804951</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.3407814845878201</c:v>
+                  <c:v>1.34078148458782</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1.32059336365173</c:v>
@@ -852,11 +847,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="206627792"/>
-        <c:axId val="206628336"/>
+        <c:axId val="2074842280"/>
+        <c:axId val="2074847752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="206627792"/>
+        <c:axId val="2074842280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -885,7 +880,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="206628336"/>
+        <c:crossAx val="2074847752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -893,7 +888,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="206628336"/>
+        <c:axId val="2074847752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -923,7 +918,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="206627792"/>
+        <c:crossAx val="2074842280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -949,7 +944,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1043,34 +1038,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1082,34 +1077,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>6.0334384479734497</c:v>
+                  <c:v>6.03343844797345</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.4853849221091604</c:v>
+                  <c:v>4.48538492210916</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.1208882472432702</c:v>
+                  <c:v>4.12088824724327</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.6550617872302502</c:v>
+                  <c:v>3.65506178723025</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.8645164337607998</c:v>
+                  <c:v>3.8645164337608</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>3.58872684596846</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.3535327558750199</c:v>
+                  <c:v>3.35353275587502</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.3378163267022498</c:v>
+                  <c:v>3.33781632670225</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.2808954856322501</c:v>
+                  <c:v>3.28089548563225</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.1486182890683798</c:v>
+                  <c:v>3.14861828906838</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1143,34 +1138,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1182,13 +1177,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.5469206057874401</c:v>
+                  <c:v>1.54692060578744</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.54490125842604</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5359077051357299</c:v>
+                  <c:v>1.53590770513573</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.52368839338786</c:v>
@@ -1200,16 +1195,16 @@
                   <c:v>1.5253718787824</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.5524189697105699</c:v>
+                  <c:v>1.55241896971057</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.5056966154706599</c:v>
+                  <c:v>1.50569661547066</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.5804717304370699</c:v>
+                  <c:v>1.58047173043707</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.5275136858198399</c:v>
+                  <c:v>1.52751368581984</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1226,11 +1221,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="212103232"/>
-        <c:axId val="27051872"/>
+        <c:axId val="2074889368"/>
+        <c:axId val="2074894840"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="212103232"/>
+        <c:axId val="2074889368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1259,7 +1254,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="27051872"/>
+        <c:crossAx val="2074894840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1267,7 +1262,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="27051872"/>
+        <c:axId val="2074894840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1297,7 +1292,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="212103232"/>
+        <c:crossAx val="2074889368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1323,7 +1318,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1683,7 +1678,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1693,17 +1688,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1718,7 +1713,7 @@
       <c r="I1" s="2"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -1735,7 +1730,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21">
       <c r="E3">
         <v>1</v>
       </c>
@@ -1779,7 +1774,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1838,7 +1833,7 @@
         <v>1.2502568118358699</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1894,7 +1889,7 @@
         <v>1.2928288976856599</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1944,7 +1939,7 @@
         <v>1.3716358886537301</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1991,7 +1986,7 @@
         <v>1.29930606218373</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -2041,7 +2036,7 @@
         <v>3.1486182890683798</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -2085,7 +2080,7 @@
         <v>1.5275136858198399</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -2096,7 +2091,7 @@
         <v>1.10113980595296</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -2107,7 +2102,7 @@
         <v>1.1002654650674299</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -2118,7 +2113,7 @@
         <v>1.1779659898652199</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -2135,8 +2130,8 @@
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Added new 350 node result
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25516"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sanchit\workspace\Bellman-Ford\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12440"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -222,8 +227,8 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.0547953345719426"/>
-                  <c:y val="0.0425269645608629"/>
+                  <c:x val="-5.4795334571942599E-2"/>
+                  <c:y val="4.2526964560862898E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -269,34 +274,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>25.0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -308,34 +313,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.34370480721398</c:v>
+                  <c:v>1.3437048072139799</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.26327805810038</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.30486805719736</c:v>
+                  <c:v>1.3048680571973601</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.29710107749564</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.25498146200484</c:v>
+                  <c:v>1.2549814620048401</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1.24970077963656</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.24621578355748</c:v>
+                  <c:v>1.2462157835574801</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.24239764811306</c:v>
+                  <c:v>1.2423976481130601</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1.24880946355503</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.25025681183587</c:v>
+                  <c:v>1.2502568118358699</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -369,34 +374,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>25.0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -408,34 +413,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.29282889768566</c:v>
+                  <c:v>1.2928288976856599</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.29282889768566</c:v>
+                  <c:v>1.2928288976856599</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.29282889768566</c:v>
+                  <c:v>1.2928288976856599</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.29282889768566</c:v>
+                  <c:v>1.2928288976856599</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.29282889768566</c:v>
+                  <c:v>1.2928288976856599</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.29282889768566</c:v>
+                  <c:v>1.2928288976856599</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.29282889768566</c:v>
+                  <c:v>1.2928288976856599</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.29282889768566</c:v>
+                  <c:v>1.2928288976856599</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.29282889768566</c:v>
+                  <c:v>1.2928288976856599</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.29282889768566</c:v>
+                  <c:v>1.2928288976856599</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -452,11 +457,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2074780904"/>
-        <c:axId val="2074786424"/>
+        <c:axId val="455473568"/>
+        <c:axId val="455465952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2074780904"/>
+        <c:axId val="455473568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -485,7 +490,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2074786424"/>
+        <c:crossAx val="455465952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -493,7 +498,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2074786424"/>
+        <c:axId val="455465952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -523,7 +528,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2074780904"/>
+        <c:crossAx val="455473568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -549,7 +554,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -617,8 +622,8 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.0547953345719426"/>
-                  <c:y val="0.0425269645608629"/>
+                  <c:x val="-5.4795334571942599E-2"/>
+                  <c:y val="4.2526964560862898E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -664,34 +669,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>25.0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -703,34 +708,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.44221246006114</c:v>
+                  <c:v>1.4422124600611399</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.39431699855319</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.33599696674708</c:v>
+                  <c:v>1.3359969667470799</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.30752097755763</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.45483309096827</c:v>
+                  <c:v>1.4548330909682701</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.39195477506776</c:v>
+                  <c:v>1.3919547750677601</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.36457429789238</c:v>
+                  <c:v>1.3645742978923801</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.25749777322223</c:v>
+                  <c:v>1.2574977732222301</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.42843014032757</c:v>
+                  <c:v>1.4284301403275701</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.37163588865373</c:v>
+                  <c:v>1.3716358886537301</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -764,34 +769,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>25.0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -803,28 +808,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.33682740305212</c:v>
+                  <c:v>1.3368274030521199</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.31430287514406</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.29165859867737</c:v>
+                  <c:v>1.2916585986773701</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.19712945639231</c:v>
+                  <c:v>1.1971294563923101</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.25842312748113</c:v>
+                  <c:v>1.2584231274811299</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.32610409708574</c:v>
+                  <c:v>1.3261040970857401</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.27124003804951</c:v>
+                  <c:v>1.2712400380495099</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.34078148458782</c:v>
+                  <c:v>1.3407814845878201</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1.32059336365173</c:v>
@@ -847,11 +852,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2074842280"/>
-        <c:axId val="2074847752"/>
+        <c:axId val="471203984"/>
+        <c:axId val="471204528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2074842280"/>
+        <c:axId val="471203984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -880,7 +885,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2074847752"/>
+        <c:crossAx val="471204528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -888,7 +893,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2074847752"/>
+        <c:axId val="471204528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -918,7 +923,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2074842280"/>
+        <c:crossAx val="471203984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -944,7 +949,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -994,7 +999,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$10</c:f>
+              <c:f>Sheet1!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1016,7 +1021,6 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:dLblPos val="t"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -1031,45 +1035,6 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$L$3:$U$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>25.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$L$10:$U$10</c:f>
@@ -1077,34 +1042,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>6.03343844797345</c:v>
+                  <c:v>1.7432039164648001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.48538492210916</c:v>
+                  <c:v>1.4856809842563701</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.12088824724327</c:v>
+                  <c:v>1.45240555106147</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.65506178723025</c:v>
+                  <c:v>1.46538313485802</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.8645164337608</c:v>
+                  <c:v>1.47191711977872</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.58872684596846</c:v>
+                  <c:v>1.4482665388335501</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.35353275587502</c:v>
+                  <c:v>1.44478059256847</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.33781632670225</c:v>
+                  <c:v>1.4577546370241901</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.28089548563225</c:v>
+                  <c:v>1.44853351425225</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.14861828906838</c:v>
+                  <c:v>1.4174839555005301</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1116,7 +1081,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$11</c:f>
+              <c:f>Sheet1!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1131,45 +1096,6 @@
           <c:dLbls>
             <c:delete val="1"/>
           </c:dLbls>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$L$3:$U$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>25.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$L$11:$U$11</c:f>
@@ -1177,34 +1103,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.54692060578744</c:v>
+                  <c:v>1.42981194919286</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.54490125842604</c:v>
+                  <c:v>1.42981194919286</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.53590770513573</c:v>
+                  <c:v>1.42981194919286</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.52368839338786</c:v>
+                  <c:v>1.42981194919286</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.5849350436401</c:v>
+                  <c:v>1.42981194919286</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.5253718787824</c:v>
+                  <c:v>1.42981194919286</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.55241896971057</c:v>
+                  <c:v>1.42981194919286</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.50569661547066</c:v>
+                  <c:v>1.42981194919286</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.58047173043707</c:v>
+                  <c:v>1.42981194919286</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.52751368581984</c:v>
+                  <c:v>1.42981194919286</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1221,11 +1147,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2074889368"/>
-        <c:axId val="2074894840"/>
+        <c:axId val="471202896"/>
+        <c:axId val="471202352"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2074889368"/>
+        <c:axId val="471202896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1254,7 +1180,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2074894840"/>
+        <c:crossAx val="471202352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1262,7 +1188,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2074894840"/>
+        <c:axId val="471202352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1292,7 +1218,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2074889368"/>
+        <c:crossAx val="471202896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1318,7 +1244,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1678,7 +1604,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1688,17 +1614,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1713,7 +1639,7 @@
       <c r="I1" s="2"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -1730,7 +1656,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E3">
         <v>1</v>
       </c>
@@ -1774,7 +1700,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1833,7 +1759,7 @@
         <v>1.2502568118358699</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1889,7 +1815,7 @@
         <v>1.2928288976856599</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1939,7 +1865,7 @@
         <v>1.3716358886537301</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1986,7 +1912,7 @@
         <v>1.29930606218373</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -2006,37 +1932,37 @@
         <v>9</v>
       </c>
       <c r="L10">
-        <v>6.0334384479734497</v>
+        <v>1.7432039164648001</v>
       </c>
       <c r="M10">
-        <v>4.4853849221091604</v>
+        <v>1.4856809842563701</v>
       </c>
       <c r="N10">
-        <v>4.1208882472432702</v>
+        <v>1.45240555106147</v>
       </c>
       <c r="O10">
-        <v>3.6550617872302502</v>
+        <v>1.46538313485802</v>
       </c>
       <c r="P10">
-        <v>3.8645164337607998</v>
+        <v>1.47191711977872</v>
       </c>
       <c r="Q10">
-        <v>3.58872684596846</v>
+        <v>1.4482665388335501</v>
       </c>
       <c r="R10">
-        <v>3.3535327558750199</v>
+        <v>1.44478059256847</v>
       </c>
       <c r="S10">
-        <v>3.3378163267022498</v>
+        <v>1.4577546370241901</v>
       </c>
       <c r="T10">
-        <v>3.2808954856322501</v>
+        <v>1.44853351425225</v>
       </c>
       <c r="U10">
-        <v>3.1486182890683798</v>
+        <v>1.4174839555005301</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -2050,37 +1976,37 @@
         <v>1.1064544729224499</v>
       </c>
       <c r="L11">
-        <v>1.5469206057874401</v>
+        <v>1.42981194919286</v>
       </c>
       <c r="M11">
-        <v>1.54490125842604</v>
+        <v>1.42981194919286</v>
       </c>
       <c r="N11">
-        <v>1.5359077051357299</v>
+        <v>1.42981194919286</v>
       </c>
       <c r="O11">
-        <v>1.52368839338786</v>
+        <v>1.42981194919286</v>
       </c>
       <c r="P11">
-        <v>1.5849350436401</v>
+        <v>1.42981194919286</v>
       </c>
       <c r="Q11">
-        <v>1.5253718787824</v>
+        <v>1.42981194919286</v>
       </c>
       <c r="R11">
-        <v>1.5524189697105699</v>
+        <v>1.42981194919286</v>
       </c>
       <c r="S11">
-        <v>1.5056966154706599</v>
+        <v>1.42981194919286</v>
       </c>
       <c r="T11">
-        <v>1.5804717304370699</v>
+        <v>1.42981194919286</v>
       </c>
       <c r="U11">
-        <v>1.5275136858198399</v>
+        <v>1.42981194919286</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -2091,7 +2017,7 @@
         <v>1.10113980595296</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -2102,7 +2028,7 @@
         <v>1.1002654650674299</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -2113,7 +2039,7 @@
         <v>1.1779659898652199</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Added Line heuristic for coefficient
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sanchit\workspace\Bellman-Ford\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antuan\SkyDrive\Documents\Masters\CS_6104\Bellman-Ford\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
   <si>
     <t>SYNTHETIC</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>Synthetic 1D</t>
+  </si>
+  <si>
+    <t>1D Synthetic Line</t>
+  </si>
+  <si>
+    <t>HeurisitcOnline/Offline</t>
   </si>
 </sst>
 </file>
@@ -463,11 +469,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1212489936"/>
-        <c:axId val="-1212494288"/>
+        <c:axId val="-1673483616"/>
+        <c:axId val="-1673763248"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1212489936"/>
+        <c:axId val="-1673483616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -496,7 +502,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1212494288"/>
+        <c:crossAx val="-1673763248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -504,7 +510,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1212494288"/>
+        <c:axId val="-1673763248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -534,7 +540,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1212489936"/>
+        <c:crossAx val="-1673483616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -858,11 +864,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1212483952"/>
-        <c:axId val="-1212487760"/>
+        <c:axId val="-1503496192"/>
+        <c:axId val="-1503497280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1212483952"/>
+        <c:axId val="-1503496192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -891,7 +897,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1212487760"/>
+        <c:crossAx val="-1503497280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -899,7 +905,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1212487760"/>
+        <c:axId val="-1503497280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -929,7 +935,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1212483952"/>
+        <c:crossAx val="-1503496192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1153,11 +1159,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1212491024"/>
-        <c:axId val="-1212490480"/>
+        <c:axId val="-1503494016"/>
+        <c:axId val="-1503499456"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1212491024"/>
+        <c:axId val="-1503494016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1186,7 +1192,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1212490480"/>
+        <c:crossAx val="-1503499456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1194,7 +1200,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1212490480"/>
+        <c:axId val="-1503499456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1224,7 +1230,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1212491024"/>
+        <c:crossAx val="-1503494016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1453,11 +1459,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1059162288"/>
-        <c:axId val="-1059166640"/>
+        <c:axId val="-1503493472"/>
+        <c:axId val="-1503503264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1059162288"/>
+        <c:axId val="-1503493472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1486,7 +1492,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1059166640"/>
+        <c:crossAx val="-1503503264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1494,7 +1500,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1059166640"/>
+        <c:axId val="-1503503264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1524,7 +1530,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1059162288"/>
+        <c:crossAx val="-1503493472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1754,11 +1760,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1213039552"/>
-        <c:axId val="-1213038464"/>
+        <c:axId val="-1503497824"/>
+        <c:axId val="-1503502720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1213039552"/>
+        <c:axId val="-1503497824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1787,7 +1793,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1213038464"/>
+        <c:crossAx val="-1503502720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1795,7 +1801,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1213038464"/>
+        <c:axId val="-1503502720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1825,7 +1831,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1213039552"/>
+        <c:crossAx val="-1503497824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1855,6 +1861,2722 @@
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>1D</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Synthetic Data Base</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$72</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Online/Offline</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$70:$H$70</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>350</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$72:$H$72</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.2633949461862399</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.15947959290735</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3988742606372799</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.27229905035391</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5390260378285401</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.4090713942975399</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.3623248511419801</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$73</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Greedy/Offline</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$70:$H$70</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>350</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$73:$H$73</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.2633949461862399</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1759071900714899</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3852318259873999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.449734250233</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.37960574797347</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.4263454302093499</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.2482744319696599</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="-1673483072"/>
+        <c:axId val="-1673482528"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$74</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>HeurisitcOnline/Offline</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$70:$H$70</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>150</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>200</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>250</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>300</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>350</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$74:$H$74</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>1.8301912851322399</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1.2461869246791599</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1.5021914541033601</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1.6153544849196999</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1.6850860907866401</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>1.68013199212305</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>1.53453959978532</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$75</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Greedy/Offline</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent4"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$70:$H$70</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>150</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>200</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>250</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>300</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>350</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$75:$H$75</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>1.3336786133554299</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1.2067683486752201</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1.1767101860025699</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1.33797772928207</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1.23333697353572</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>1.58826973229016</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>1.5957218431342399</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-1673483072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of Nodes</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1673482528"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1673482528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Competitive Ratio</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1673483072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.75901676239745397"/>
+          <c:y val="0.54625554706338919"/>
+          <c:w val="0.17079355116842279"/>
+          <c:h val="0.12697605801532147"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>1D</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Synthetic Data Heuristic Line</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$74</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>HeurisitcOnline/Offline</c:v>
+                </c:pt>
+              </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$70:$H$70</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>350</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$74:$H$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.8301912851322399</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2461869246791599</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5021914541033601</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.6153544849196999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.6850860907866401</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.68013199212305</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.53453959978532</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$75</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Greedy/Offline</c:v>
+                </c:pt>
+              </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$70:$H$70</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>350</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$75:$H$75</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.3336786133554299</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2067683486752201</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1767101860025699</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.33797772928207</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.23333697353572</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.58826973229016</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5957218431342399</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="-1428672304"/>
+        <c:axId val="-1428667408"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$72</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Online/Offline</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$70:$H$70</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>150</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>200</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>250</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>300</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>350</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$72:$H$72</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>1.2633949461862399</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1.15947959290735</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1.3988742606372799</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1.27229905035391</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1.5390260378285401</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>1.4090713942975399</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>1.3623248511419801</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$73</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Greedy/Offline</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$70:$H$70</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>150</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>200</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>250</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>300</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>350</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$73:$H$73</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>1.2633949461862399</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1.1759071900714899</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1.3852318259873999</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1.449734250233</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1.37960574797347</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>1.4263454302093499</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>1.2482744319696599</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-1428672304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of Nodes</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1428667408"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1428667408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Competitive Ratio</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1428672304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.75901676239745397"/>
+          <c:y val="0.54625554706338919"/>
+          <c:w val="0.19696102298806853"/>
+          <c:h val="0.23608064793255246"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2012,6 +4734,68 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>449580</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2283,19 +5067,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U17"/>
+  <dimension ref="A1:U75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X10" sqref="X10"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F82" sqref="F82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2310,7 +5094,7 @@
       <c r="I1" s="2"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -2327,7 +5111,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="E3">
         <v>1</v>
       </c>
@@ -2371,7 +5155,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -2430,7 +5214,7 @@
         <v>1.2502568118358699</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -2486,7 +5270,7 @@
         <v>1.2928288976856599</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -2536,7 +5320,7 @@
         <v>1.2437499632367099</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -2583,7 +5367,7 @@
         <v>1.24978199559117</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -2633,7 +5417,7 @@
         <v>1.4174839555005301</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -2677,7 +5461,7 @@
         <v>1.42981194919286</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -2721,7 +5505,7 @@
         <v>1.79489164354724</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -2762,7 +5546,7 @@
         <v>1.68621213417752</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -2806,7 +5590,7 @@
         <v>1.3704489421478101</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -2845,6 +5629,138 @@
       </c>
       <c r="U17">
         <v>1.3716530015480699</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B70">
+        <v>50</v>
+      </c>
+      <c r="C70">
+        <v>100</v>
+      </c>
+      <c r="D70">
+        <v>150</v>
+      </c>
+      <c r="E70">
+        <v>200</v>
+      </c>
+      <c r="F70">
+        <v>250</v>
+      </c>
+      <c r="G70">
+        <v>300</v>
+      </c>
+      <c r="H70">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>4</v>
+      </c>
+      <c r="B72">
+        <v>1.2633949461862399</v>
+      </c>
+      <c r="C72">
+        <v>1.15947959290735</v>
+      </c>
+      <c r="D72">
+        <v>1.3988742606372799</v>
+      </c>
+      <c r="E72">
+        <v>1.27229905035391</v>
+      </c>
+      <c r="F72">
+        <v>1.5390260378285401</v>
+      </c>
+      <c r="G72">
+        <v>1.4090713942975399</v>
+      </c>
+      <c r="H72">
+        <v>1.3623248511419801</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>5</v>
+      </c>
+      <c r="B73">
+        <v>1.2633949461862399</v>
+      </c>
+      <c r="C73">
+        <v>1.1759071900714899</v>
+      </c>
+      <c r="D73">
+        <v>1.3852318259873999</v>
+      </c>
+      <c r="E73">
+        <v>1.449734250233</v>
+      </c>
+      <c r="F73">
+        <v>1.37960574797347</v>
+      </c>
+      <c r="G73">
+        <v>1.4263454302093499</v>
+      </c>
+      <c r="H73">
+        <v>1.2482744319696599</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>13</v>
+      </c>
+      <c r="B74">
+        <v>1.8301912851322399</v>
+      </c>
+      <c r="C74">
+        <v>1.2461869246791599</v>
+      </c>
+      <c r="D74">
+        <v>1.5021914541033601</v>
+      </c>
+      <c r="E74">
+        <v>1.6153544849196999</v>
+      </c>
+      <c r="F74">
+        <v>1.6850860907866401</v>
+      </c>
+      <c r="G74">
+        <v>1.68013199212305</v>
+      </c>
+      <c r="H74">
+        <v>1.53453959978532</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>5</v>
+      </c>
+      <c r="B75">
+        <v>1.3336786133554299</v>
+      </c>
+      <c r="C75">
+        <v>1.2067683486752201</v>
+      </c>
+      <c r="D75">
+        <v>1.1767101860025699</v>
+      </c>
+      <c r="E75">
+        <v>1.33797772928207</v>
+      </c>
+      <c r="F75">
+        <v>1.23333697353572</v>
+      </c>
+      <c r="G75">
+        <v>1.58826973229016</v>
+      </c>
+      <c r="H75">
+        <v>1.5957218431342399</v>
       </c>
     </row>
   </sheetData>

</xml_diff>